<commit_message>
include pests in matrix
</commit_message>
<xml_diff>
--- a/companion-plants.xlsx
+++ b/companion-plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arcarter/code/plant-guilds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B04F72-70A4-EA4B-8B35-00882E2C9A37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F9E402-5588-6749-BDDD-3E2BBB439F63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{E5B86D71-C82A-E84B-872D-5A6E11613994}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{E5B86D71-C82A-E84B-872D-5A6E11613994}"/>
   </bookViews>
   <sheets>
     <sheet name="Vegetables" sheetId="2" r:id="rId1"/>
@@ -8618,7 +8618,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> slugs (see Garlic), aphids,</t>
+      <t xml:space="preserve"> slugs, aphids,</t>
     </r>
     <r>
       <rPr>
@@ -9128,8 +9128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8559685-2A6B-0A40-AD38-A3BAABEEFD35}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10134,7 +10134,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10563,7 +10563,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11338,8 +11338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F83275-BE02-1E4C-B80A-87DE7EAB73F8}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11832,8 +11832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DB4BE8-C7BA-C141-8692-5ADA62E09D8E}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>